<commit_message>
Lab 4 decrypt monoalphabet
</commit_message>
<xml_diff>
--- a/KMZI_Lab4/Graphics_Lab4.xlsx
+++ b/KMZI_Lab4/Graphics_Lab4.xlsx
@@ -5,28 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valda\source\repos\semester#6\КМЗИ\KMZI_Lab2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valda\source\repos\semester#6\КМЗИ\KMZI_Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36503F00-AD54-4D9A-9B36-3053B0DD4B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2988822-C658-4200-8E5F-F91AC544A245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12200" xr2:uid="{83DAACA7-D030-470B-BA63-03C67BE42085}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Моноалфавитный шифр" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$B$3:$B$30</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$B$3:$B$35</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$C$3:$C$35</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$C$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$C$3:$C$30</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$C$3:$C$35</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$E$3:$E$34</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$F$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$F$3:$F$34</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$B$3:$B$35</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$C$2</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Моноалфавитный шифр'!$B$3:$B$31</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Моноалфавитный шифр'!$C$2</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Моноалфавитный шифр'!$C$3:$C$31</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Моноалфавитный шифр'!$E$3:$E$31</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Моноалфавитный шифр'!$F$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Моноалфавитный шифр'!$F$3:$F$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>_x000D_</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Symbol</t>
   </si>
@@ -123,15 +115,9 @@
     <t>z</t>
   </si>
   <si>
-    <t>[x, 1]</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>German</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
@@ -145,6 +131,19 @@
   </si>
   <si>
     <t>ö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+;29</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Open text</t>
+  </si>
+  <si>
+    <t>Cypher text</t>
   </si>
 </sst>
 </file>
@@ -223,7 +222,7 @@
         <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -231,7 +230,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Немецкий язык</cx:v>
+          <cx:v>Открытый текст (немецкий язык)</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -251,7 +250,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Немецкий язык</a:t>
+            <a:t>Открытый текст (немецкий язык)</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -261,7 +260,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{E13C508D-FB03-4B75-BF6B-DC9E8FE8861C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Appearances</cx:v>
             </cx:txData>
           </cx:tx>
@@ -314,6 +313,97 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Шифротекст (немецкий язык)</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Шифротекст (немецкий язык)</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{3166B8A2-34BC-4EDF-848A-6202F9A588FF}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>Appearances</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:aggregation/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{20758516-59D1-4100-ABF3-78C8BEDDBF8E}">
+          <cx:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </cx:spPr>
+          <cx:axisId val="2"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2" hidden="1">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:spPr>
+    <a:ln w="9525">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+    </a:ln>
+  </cx:spPr>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -354,7 +444,521 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -866,16 +1470,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>13822</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>369255</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>12801</xdr:rowOff>
+      <xdr:rowOff>5917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>635859</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>68849</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180729</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -911,8 +1515,86 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2118349" y="198495"/>
-              <a:ext cx="7177582" cy="2772602"/>
+              <a:off x="3906369" y="186645"/>
+              <a:ext cx="5508724" cy="4873752"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-BY" sz="1100"/>
+                <a:t>Эта диаграмма недоступна в вашей версии Excel.
+Изменение этой фигуры или сохранение книги в другом формате приведет к остаточному повреждению диаграммы.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>3226</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>361457</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>8606</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Диаграмма 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7091C07-1D43-45C0-B520-011694EA05CB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9973844" y="189980"/>
+              <a:ext cx="5508131" cy="4939266"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1242,10 +1924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3BEB4A-FDC3-4F90-A17A-66968A6627E1}">
-  <dimension ref="B1:F52"/>
+  <dimension ref="B1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,259 +1940,441 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>473</v>
       </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>473</v>
+      </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>341</v>
       </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>341</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>1007</v>
       </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>1007</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>247</v>
       </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>247</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>102</v>
       </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>102</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>116</v>
       </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>116</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>456</v>
       </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>456</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>475</v>
       </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>475</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>109</v>
       </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>169</v>
       </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>169</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>221</v>
       </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>221</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>61</v>
       </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>228</v>
       </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>228</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>577</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>576</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>588</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>192</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>401</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>179</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <v>17</v>
       </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Lab 4 full code
</commit_message>
<xml_diff>
--- a/KMZI_Lab4/Graphics_Lab4.xlsx
+++ b/KMZI_Lab4/Graphics_Lab4.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valda\source\repos\semester#6\КМЗИ\KMZI_Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2988822-C658-4200-8E5F-F91AC544A245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C2A65-2F21-4108-ACEC-D53DB11549D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12200" xr2:uid="{83DAACA7-D030-470B-BA63-03C67BE42085}"/>
   </bookViews>
   <sheets>
     <sheet name="Моноалфавитный шифр" sheetId="1" r:id="rId1"/>
+    <sheet name="Шифр Трисемуса" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Моноалфавитный шифр'!$B$3:$B$31</definedName>
@@ -1927,7 +1928,7 @@
   <dimension ref="B1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2385,4 +2386,16 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF02F33E-A090-4E67-AAAB-E8C49258D1C9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>